<commit_message>
Showing good progress with voltage sources
</commit_message>
<xml_diff>
--- a/Outputs/CYME_Extract_13Bus.xlsx
+++ b/Outputs/CYME_Extract_13Bus.xlsx
@@ -1,22 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29029"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unbcloud-my.sharepoint.com/personal/ebelliv1_unb_ca/Documents/Smart Grid/Github/CYME-EXTRACT/Outputs/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="1" documentId="11_FC09968B4D7971AF3533E9B7F070FDE8B5956BF4" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6A57EC9D-93AF-4243-87E2-8AC596BAF90C}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
     <sheet name="Bus" sheetId="2" r:id="rId2"/>
-    <sheet name="Voltage_Source" sheetId="3" r:id="rId3"/>
+    <sheet name="Voltage Source" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="79">
   <si>
     <t>Excel file version</t>
   </si>
@@ -168,71 +174,98 @@
     <t>Slack</t>
   </si>
   <si>
-    <t>SourceNodeID</t>
-  </si>
-  <si>
-    <t>DeviceNumber</t>
-  </si>
-  <si>
-    <t>SourceID</t>
-  </si>
-  <si>
-    <t>DesiredVoltage_kVLL</t>
-  </si>
-  <si>
-    <t>EquivalentConfig</t>
-  </si>
-  <si>
-    <t>KVLL</t>
-  </si>
-  <si>
-    <t>OperatingVoltage1_kVLN</t>
-  </si>
-  <si>
-    <t>OperatingAngle1_deg</t>
-  </si>
-  <si>
-    <t>PosSeqR</t>
-  </si>
-  <si>
-    <t>PosSeqX</t>
-  </si>
-  <si>
-    <t>NegSeqR</t>
-  </si>
-  <si>
-    <t>NegSeqX</t>
-  </si>
-  <si>
-    <t>ZeroSeqR</t>
-  </si>
-  <si>
-    <t>ZeroSeqX</t>
-  </si>
-  <si>
-    <t>NominalCapacity1_MVA</t>
-  </si>
-  <si>
-    <t>NominalCapacity2_MVA</t>
-  </si>
-  <si>
-    <t>650</t>
-  </si>
-  <si>
-    <t>SUB650WYE-S2</t>
+    <t>Positive-Sequence Voltage Source</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>End of Positive-Sequence Voltage Source</t>
+  </si>
+  <si>
+    <t>Single-Phase Voltage Source</t>
+  </si>
+  <si>
+    <t>End of Single-Phase Voltage Source</t>
+  </si>
+  <si>
+    <t>Three-Phase Voltage Source with Short-Circuit Level Data</t>
   </si>
   <si>
     <t>SUB650WYE</t>
   </si>
   <si>
-    <t>Yg</t>
+    <t>End of Three-Phase Voltage Source Short-Circuit Level Data</t>
+  </si>
+  <si>
+    <t>Three-Phase Voltage Source with Sequential Data</t>
+  </si>
+  <si>
+    <t>End of Three-Phase Voltage Source Sequential Data</t>
+  </si>
+  <si>
+    <t>Go to Type List</t>
+  </si>
+  <si>
+    <t>Bus1</t>
+  </si>
+  <si>
+    <t>Voltage (pu)</t>
+  </si>
+  <si>
+    <t>Voltage (V)</t>
+  </si>
+  <si>
+    <t>Bus2</t>
+  </si>
+  <si>
+    <t>Angle (deg)</t>
+  </si>
+  <si>
+    <t>Bus3</t>
+  </si>
+  <si>
+    <t>Rs (pu)</t>
+  </si>
+  <si>
+    <t>Rs (Ohm)</t>
+  </si>
+  <si>
+    <t>kV (ph-ph RMS)</t>
+  </si>
+  <si>
+    <t>Xs (pu)</t>
+  </si>
+  <si>
+    <t>Xs (Ohm)</t>
+  </si>
+  <si>
+    <t>Angle_a (deg)</t>
+  </si>
+  <si>
+    <t>SC1ph (MVA)</t>
+  </si>
+  <si>
+    <t>R1 (Ohm)</t>
+  </si>
+  <si>
+    <t>SC3ph (MVA)</t>
+  </si>
+  <si>
+    <t>X1 (Ohm)</t>
+  </si>
+  <si>
+    <t>R0 (Ohm)</t>
+  </si>
+  <si>
+    <t>X0 (Ohm)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -295,13 +328,21 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -339,7 +380,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -373,6 +414,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -407,9 +449,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -582,14 +625,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -597,7 +640,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -605,7 +648,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -613,7 +656,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -627,14 +670,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F36"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -654,7 +697,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -674,7 +717,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -694,7 +737,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -714,7 +757,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -734,7 +777,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -754,7 +797,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>17</v>
       </c>
@@ -774,7 +817,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>18</v>
       </c>
@@ -794,7 +837,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>19</v>
       </c>
@@ -814,7 +857,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>20</v>
       </c>
@@ -834,7 +877,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>21</v>
       </c>
@@ -854,7 +897,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>22</v>
       </c>
@@ -874,7 +917,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>23</v>
       </c>
@@ -894,7 +937,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>24</v>
       </c>
@@ -914,7 +957,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>25</v>
       </c>
@@ -934,7 +977,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>26</v>
       </c>
@@ -954,7 +997,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>27</v>
       </c>
@@ -974,7 +1017,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>28</v>
       </c>
@@ -994,7 +1037,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>29</v>
       </c>
@@ -1014,7 +1057,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>30</v>
       </c>
@@ -1034,7 +1077,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>31</v>
       </c>
@@ -1054,7 +1097,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>32</v>
       </c>
@@ -1074,7 +1117,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>33</v>
       </c>
@@ -1094,7 +1137,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="24" spans="1:6">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>34</v>
       </c>
@@ -1114,7 +1157,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="25" spans="1:6">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>35</v>
       </c>
@@ -1134,7 +1177,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="26" spans="1:6">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>36</v>
       </c>
@@ -1154,7 +1197,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="27" spans="1:6">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>37</v>
       </c>
@@ -1174,7 +1217,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="28" spans="1:6">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>38</v>
       </c>
@@ -1194,7 +1237,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="29" spans="1:6">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>39</v>
       </c>
@@ -1214,7 +1257,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="30" spans="1:6">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>40</v>
       </c>
@@ -1234,7 +1277,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="31" spans="1:6">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>41</v>
       </c>
@@ -1254,7 +1297,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="32" spans="1:6">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>42</v>
       </c>
@@ -1274,7 +1317,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="33" spans="1:6">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>43</v>
       </c>
@@ -1294,7 +1337,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="34" spans="1:6">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>44</v>
       </c>
@@ -1314,7 +1357,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="35" spans="1:6">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>45</v>
       </c>
@@ -1334,7 +1377,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="36" spans="1:6">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>46</v>
       </c>
@@ -1360,90 +1403,192 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:P2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:J16"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="54.5703125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:16">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
         <v>50</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>51</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D2" t="s">
+        <v>65</v>
+      </c>
+      <c r="E2" t="s">
+        <v>67</v>
+      </c>
+      <c r="F2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>52</v>
       </c>
-      <c r="D1" s="1" t="s">
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>53</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="B5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>51</v>
+      </c>
+      <c r="B6" t="s">
+        <v>61</v>
+      </c>
+      <c r="C6" t="s">
+        <v>63</v>
+      </c>
+      <c r="D6" t="s">
+        <v>65</v>
+      </c>
+      <c r="E6" t="s">
+        <v>68</v>
+      </c>
+      <c r="F6" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>54</v>
       </c>
-      <c r="F1" s="1" t="s">
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>55</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="B9" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>51</v>
+      </c>
+      <c r="B10" t="s">
+        <v>61</v>
+      </c>
+      <c r="C10" t="s">
+        <v>64</v>
+      </c>
+      <c r="D10" t="s">
+        <v>66</v>
+      </c>
+      <c r="E10" t="s">
+        <v>69</v>
+      </c>
+      <c r="F10" t="s">
+        <v>72</v>
+      </c>
+      <c r="G10" t="s">
+        <v>73</v>
+      </c>
+      <c r="H10" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>56</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="B11" t="s">
+        <v>26</v>
+      </c>
+      <c r="C11" t="s">
+        <v>27</v>
+      </c>
+      <c r="D11" t="s">
+        <v>28</v>
+      </c>
+      <c r="E11">
+        <v>4.16</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>200000</v>
+      </c>
+      <c r="H11">
+        <v>200000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>57</v>
       </c>
-      <c r="I1" s="1" t="s">
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>58</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="B14" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>51</v>
+      </c>
+      <c r="B15" t="s">
+        <v>61</v>
+      </c>
+      <c r="C15" t="s">
+        <v>64</v>
+      </c>
+      <c r="D15" t="s">
+        <v>66</v>
+      </c>
+      <c r="E15" t="s">
+        <v>69</v>
+      </c>
+      <c r="F15" t="s">
+        <v>72</v>
+      </c>
+      <c r="G15" t="s">
+        <v>74</v>
+      </c>
+      <c r="H15" t="s">
+        <v>76</v>
+      </c>
+      <c r="I15" t="s">
+        <v>77</v>
+      </c>
+      <c r="J15" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>59</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16">
-      <c r="A2" t="s">
-        <v>66</v>
-      </c>
-      <c r="B2" t="s">
-        <v>67</v>
-      </c>
-      <c r="C2" t="s">
-        <v>68</v>
-      </c>
-      <c r="E2" t="s">
-        <v>69</v>
-      </c>
-      <c r="F2">
-        <v>4.16</v>
-      </c>
-      <c r="G2">
-        <v>2.401777</v>
-      </c>
-      <c r="H2">
-        <v>0</v>
-      </c>
-      <c r="O2">
-        <v>150</v>
-      </c>
-      <c r="P2">
-        <v>150</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added load page (working)
</commit_message>
<xml_diff>
--- a/Outputs/CYME_Extract_13Bus.xlsx
+++ b/Outputs/CYME_Extract_13Bus.xlsx
@@ -1,28 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29029"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unbcloud-my.sharepoint.com/personal/ebelliv1_unb_ca/Documents/Smart Grid/Github/CYME-EXTRACT/Outputs/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="11_FC09968B4D7971AF3533E9B7F070FDE8B5956BF4" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6A57EC9D-93AF-4243-87E2-8AC596BAF90C}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
     <sheet name="Bus" sheetId="2" r:id="rId2"/>
     <sheet name="Voltage Source" sheetId="3" r:id="rId3"/>
+    <sheet name="Load" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="131">
   <si>
     <t>Excel file version</t>
   </si>
@@ -174,84 +169,102 @@
     <t>Slack</t>
   </si>
   <si>
+    <t>PositiveSeqVsource</t>
+  </si>
+  <si>
+    <t>SinglePhaseVsource</t>
+  </si>
+  <si>
+    <t>ThreePhaseShortCircuitVsource</t>
+  </si>
+  <si>
+    <t>ThreePhaseSequentialVsource</t>
+  </si>
+  <si>
+    <t>Important notes:</t>
+  </si>
+  <si>
+    <t>Default order of blocks and columns after row 11 must not change</t>
+  </si>
+  <si>
+    <t>One empty row between End of each block and the next block is mandatory; otherwise, empty rows are NOT allowed</t>
+  </si>
+  <si>
     <t>Positive-Sequence Voltage Source</t>
   </si>
   <si>
+    <t>Go to Type List</t>
+  </si>
+  <si>
     <t>ID</t>
   </si>
   <si>
+    <t>Voltage (pu)</t>
+  </si>
+  <si>
+    <t>Angle (deg)</t>
+  </si>
+  <si>
+    <t>Rs (pu)</t>
+  </si>
+  <si>
+    <t>Xs (pu)</t>
+  </si>
+  <si>
     <t>End of Positive-Sequence Voltage Source</t>
   </si>
   <si>
     <t>Single-Phase Voltage Source</t>
   </si>
   <si>
+    <t>Bus1</t>
+  </si>
+  <si>
+    <t>Voltage (V)</t>
+  </si>
+  <si>
+    <t>Rs (Ohm)</t>
+  </si>
+  <si>
+    <t>Xs (Ohm)</t>
+  </si>
+  <si>
     <t>End of Single-Phase Voltage Source</t>
   </si>
   <si>
     <t>Three-Phase Voltage Source with Short-Circuit Level Data</t>
   </si>
   <si>
+    <t>Bus2</t>
+  </si>
+  <si>
+    <t>Bus3</t>
+  </si>
+  <si>
+    <t>kV (ph-ph RMS)</t>
+  </si>
+  <si>
+    <t>Angle_a (deg)</t>
+  </si>
+  <si>
+    <t>SC1ph (MVA)</t>
+  </si>
+  <si>
+    <t>SC3ph (MVA)</t>
+  </si>
+  <si>
     <t>SUB650WYE</t>
   </si>
   <si>
-    <t>End of Three-Phase Voltage Source Short-Circuit Level Data</t>
+    <t>End of Three-Phase Voltage Source with Short-Circuit Level Data</t>
   </si>
   <si>
     <t>Three-Phase Voltage Source with Sequential Data</t>
   </si>
   <si>
-    <t>End of Three-Phase Voltage Source Sequential Data</t>
-  </si>
-  <si>
-    <t>Go to Type List</t>
-  </si>
-  <si>
-    <t>Bus1</t>
-  </si>
-  <si>
-    <t>Voltage (pu)</t>
-  </si>
-  <si>
-    <t>Voltage (V)</t>
-  </si>
-  <si>
-    <t>Bus2</t>
-  </si>
-  <si>
-    <t>Angle (deg)</t>
-  </si>
-  <si>
-    <t>Bus3</t>
-  </si>
-  <si>
-    <t>Rs (pu)</t>
-  </si>
-  <si>
-    <t>Rs (Ohm)</t>
-  </si>
-  <si>
-    <t>kV (ph-ph RMS)</t>
-  </si>
-  <si>
-    <t>Xs (pu)</t>
-  </si>
-  <si>
-    <t>Xs (Ohm)</t>
-  </si>
-  <si>
-    <t>Angle_a (deg)</t>
-  </si>
-  <si>
-    <t>SC1ph (MVA)</t>
-  </si>
-  <si>
     <t>R1 (Ohm)</t>
   </si>
   <si>
-    <t>SC3ph (MVA)</t>
-  </si>
-  <si>
     <t>X1 (Ohm)</t>
   </si>
   <si>
@@ -259,13 +272,154 @@
   </si>
   <si>
     <t>X0 (Ohm)</t>
+  </si>
+  <si>
+    <t>End of Three-Phase Voltage Source with Sequential Data</t>
+  </si>
+  <si>
+    <t>PositiveSeqZload</t>
+  </si>
+  <si>
+    <t>ThreePhaseZIPLoad</t>
+  </si>
+  <si>
+    <t>PositiveSeqPload</t>
+  </si>
+  <si>
+    <t>PositiveSeqIload</t>
+  </si>
+  <si>
+    <t>SinglePhaseZIPLoad</t>
+  </si>
+  <si>
+    <t>TwoPhaseZIPLoad</t>
+  </si>
+  <si>
+    <t>Positive-Sequence Constant Impedance Load</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>P (MW)</t>
+  </si>
+  <si>
+    <t>Q (MVAr)</t>
+  </si>
+  <si>
+    <t>End of Positive-Sequence Constant Impedance Load</t>
+  </si>
+  <si>
+    <t>Positive-Sequence Constant Power Load</t>
+  </si>
+  <si>
+    <t>End of Positive-Sequence Constant Power Load</t>
+  </si>
+  <si>
+    <t>Positive-Sequence Constant Current Load</t>
+  </si>
+  <si>
+    <t>End of Positive-Sequence Constant Current Load</t>
+  </si>
+  <si>
+    <t>Single-Phase ZIP Load</t>
+  </si>
+  <si>
+    <t>V (kV)</t>
+  </si>
+  <si>
+    <t>Bandwidth (pu)</t>
+  </si>
+  <si>
+    <t>Conn. type</t>
+  </si>
+  <si>
+    <t>K_z</t>
+  </si>
+  <si>
+    <t>K_i</t>
+  </si>
+  <si>
+    <t>K_p</t>
+  </si>
+  <si>
+    <t>Use initial voltage?</t>
+  </si>
+  <si>
+    <t>P1 (kW)</t>
+  </si>
+  <si>
+    <t>Q1 (kVAr)</t>
+  </si>
+  <si>
+    <t>LD_645</t>
+  </si>
+  <si>
+    <t>wye</t>
+  </si>
+  <si>
+    <t>LD_652</t>
+  </si>
+  <si>
+    <t>LD_611</t>
+  </si>
+  <si>
+    <t>End of SinglePhase ZIP Load</t>
+  </si>
+  <si>
+    <t>Two-Phase ZIP Load</t>
+  </si>
+  <si>
+    <t>P1(kW)</t>
+  </si>
+  <si>
+    <t>Q1(kVAr)</t>
+  </si>
+  <si>
+    <t>P2 (kW)</t>
+  </si>
+  <si>
+    <t>Q2 (kVAr)</t>
+  </si>
+  <si>
+    <t>LD_692</t>
+  </si>
+  <si>
+    <t>LD_646</t>
+  </si>
+  <si>
+    <t>End of TwoPhase ZIP Load</t>
+  </si>
+  <si>
+    <t>Three-Phase ZIP Load</t>
+  </si>
+  <si>
+    <t>P3 (kW)</t>
+  </si>
+  <si>
+    <t>Q3 (kVAr)</t>
+  </si>
+  <si>
+    <t>LD_675</t>
+  </si>
+  <si>
+    <t>LD_634</t>
+  </si>
+  <si>
+    <t>LD_671</t>
+  </si>
+  <si>
+    <t>End of Three-Phase ZIP Load</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.00"/>
+  </numFmts>
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -281,16 +435,45 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFF00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFFFF00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF595959"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -313,36 +496,46 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2007 - 2010">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -380,7 +573,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2007 - 2010">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -414,7 +607,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -449,10 +641,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2007 - 2010">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -625,14 +816,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -640,7 +831,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -648,7 +839,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -656,7 +847,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -670,14 +861,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F36"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -697,7 +888,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -717,7 +908,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -737,7 +928,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -757,7 +948,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -777,7 +968,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -797,7 +988,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6">
       <c r="A7" t="s">
         <v>17</v>
       </c>
@@ -817,7 +1008,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6">
       <c r="A8" t="s">
         <v>18</v>
       </c>
@@ -837,7 +1028,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6">
       <c r="A9" t="s">
         <v>19</v>
       </c>
@@ -857,7 +1048,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6">
       <c r="A10" t="s">
         <v>20</v>
       </c>
@@ -877,7 +1068,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6">
       <c r="A11" t="s">
         <v>21</v>
       </c>
@@ -897,7 +1088,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6">
       <c r="A12" t="s">
         <v>22</v>
       </c>
@@ -917,7 +1108,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6">
       <c r="A13" t="s">
         <v>23</v>
       </c>
@@ -937,7 +1128,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6">
       <c r="A14" t="s">
         <v>24</v>
       </c>
@@ -957,7 +1148,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6">
       <c r="A15" t="s">
         <v>25</v>
       </c>
@@ -977,7 +1168,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6">
       <c r="A16" t="s">
         <v>26</v>
       </c>
@@ -997,7 +1188,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6">
       <c r="A17" t="s">
         <v>27</v>
       </c>
@@ -1017,7 +1208,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6">
       <c r="A18" t="s">
         <v>28</v>
       </c>
@@ -1037,7 +1228,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6">
       <c r="A19" t="s">
         <v>29</v>
       </c>
@@ -1057,7 +1248,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6">
       <c r="A20" t="s">
         <v>30</v>
       </c>
@@ -1077,7 +1268,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6">
       <c r="A21" t="s">
         <v>31</v>
       </c>
@@ -1097,7 +1288,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6">
       <c r="A22" t="s">
         <v>32</v>
       </c>
@@ -1117,7 +1308,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6">
       <c r="A23" t="s">
         <v>33</v>
       </c>
@@ -1137,7 +1328,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6">
       <c r="A24" t="s">
         <v>34</v>
       </c>
@@ -1157,7 +1348,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6">
       <c r="A25" t="s">
         <v>35</v>
       </c>
@@ -1177,7 +1368,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6">
       <c r="A26" t="s">
         <v>36</v>
       </c>
@@ -1197,7 +1388,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6">
       <c r="A27" t="s">
         <v>37</v>
       </c>
@@ -1217,7 +1408,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6">
       <c r="A28" t="s">
         <v>38</v>
       </c>
@@ -1237,7 +1428,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6">
       <c r="A29" t="s">
         <v>39</v>
       </c>
@@ -1257,7 +1448,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6">
       <c r="A30" t="s">
         <v>40</v>
       </c>
@@ -1277,7 +1468,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6">
       <c r="A31" t="s">
         <v>41</v>
       </c>
@@ -1297,7 +1488,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6">
       <c r="A32" t="s">
         <v>42</v>
       </c>
@@ -1317,7 +1508,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6">
       <c r="A33" t="s">
         <v>43</v>
       </c>
@@ -1337,7 +1528,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6">
       <c r="A34" t="s">
         <v>44</v>
       </c>
@@ -1357,7 +1548,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6">
       <c r="A35" t="s">
         <v>45</v>
       </c>
@@ -1377,7 +1568,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6">
       <c r="A36" t="s">
         <v>46</v>
       </c>
@@ -1403,195 +1594,1081 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:J16"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:J26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="54.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.7109375" customWidth="1"/>
+    <col min="2" max="4" width="14.7109375" customWidth="1"/>
+    <col min="5" max="5" width="18.7109375" customWidth="1"/>
+    <col min="6" max="6" width="14.7109375" customWidth="1"/>
+    <col min="7" max="8" width="16.7109375" customWidth="1"/>
+    <col min="9" max="10" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:8">
+      <c r="A1" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="B1" t="s">
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" s="3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="5"/>
+      <c r="H9" s="5"/>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B10" s="5"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="5"/>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" s="6" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>51</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="D12" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="A15" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="A16" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="F16" s="6" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10">
+      <c r="A17" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10">
+      <c r="A19" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B19" s="2"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10">
+      <c r="A20" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="E20" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="F20" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="G20" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="H20" s="6" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10">
+      <c r="A21" t="s">
+        <v>78</v>
+      </c>
+      <c r="B21" t="s">
+        <v>26</v>
+      </c>
+      <c r="C21" t="s">
+        <v>27</v>
+      </c>
+      <c r="D21" t="s">
+        <v>28</v>
+      </c>
+      <c r="E21" s="7">
+        <v>4.16</v>
+      </c>
+      <c r="F21" s="7">
+        <v>0</v>
+      </c>
+      <c r="G21" s="8">
+        <v>200000</v>
+      </c>
+      <c r="H21" s="8">
+        <v>200000</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10">
+      <c r="A22" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10">
+      <c r="A24" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B24" s="2"/>
+      <c r="C24" s="2"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10">
+      <c r="A25" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="B25" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="C25" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="D25" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="E25" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="F25" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="G25" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="H25" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="I25" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="J25" s="6" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10">
+      <c r="A26" t="s">
+        <v>85</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="11">
+    <mergeCell ref="A8:H8"/>
+    <mergeCell ref="A9:H9"/>
+    <mergeCell ref="A10:H10"/>
+    <mergeCell ref="A11:D11"/>
+    <mergeCell ref="A13:D13"/>
+    <mergeCell ref="A15:D15"/>
+    <mergeCell ref="A17:D17"/>
+    <mergeCell ref="A19:D19"/>
+    <mergeCell ref="A22:D22"/>
+    <mergeCell ref="A24:D24"/>
+    <mergeCell ref="A26:D26"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="A2" location="'Voltage Source'!A12:F13" display="PositiveSeqVsource"/>
+    <hyperlink ref="A3" location="'Voltage Source'!A16:F17" display="SinglePhaseVsource"/>
+    <hyperlink ref="A4" location="'Voltage Source'!A20:H22" display="ThreePhaseShortCircuitVsource"/>
+    <hyperlink ref="A5" location="'Voltage Source'!A25:J26" display="ThreePhaseSequentialVsource"/>
+    <hyperlink ref="E11" location="'Voltage Source'!A1" display="Go to Type List"/>
+    <hyperlink ref="E15" location="'Voltage Source'!A1" display="Go to Type List"/>
+    <hyperlink ref="E19" location="'Voltage Source'!A1" display="Go to Type List"/>
+    <hyperlink ref="E24" location="'Voltage Source'!A1" display="Go to Type List"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:R41"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="28.7109375" customWidth="1"/>
+    <col min="2" max="3" width="10.7109375" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" customWidth="1"/>
+    <col min="5" max="5" width="14.7109375" customWidth="1"/>
+    <col min="6" max="8" width="9.7109375" customWidth="1"/>
+    <col min="9" max="9" width="18.7109375" customWidth="1"/>
+    <col min="10" max="12" width="14.7109375" customWidth="1"/>
+    <col min="13" max="18" width="10.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="A1" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" s="3" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" s="3" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" s="3" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" s="3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="5"/>
+      <c r="H9" s="5"/>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B10" s="5"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="5"/>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="C12" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C2" t="s">
-        <v>62</v>
-      </c>
-      <c r="D2" t="s">
-        <v>65</v>
-      </c>
-      <c r="E2" t="s">
-        <v>67</v>
-      </c>
-      <c r="F2" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>53</v>
-      </c>
-      <c r="B5" t="s">
+      <c r="D12" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="A15" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="A16" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15">
+      <c r="A17" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15">
+      <c r="A19" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="B19" s="2"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15">
+      <c r="A20" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="E20" s="6" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15">
+      <c r="A21" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15">
+      <c r="A23" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="B23" s="2"/>
+      <c r="C23" s="2"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15">
+      <c r="A24" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="D24" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="E24" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="F24" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="G24" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="H24" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="I24" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="J24" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="K24" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="L24" s="6" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15">
+      <c r="A25" t="s">
+        <v>111</v>
+      </c>
+      <c r="B25" s="8">
+        <v>1</v>
+      </c>
+      <c r="C25" s="7">
+        <v>4.16</v>
+      </c>
+      <c r="D25" s="7">
+        <v>0.2</v>
+      </c>
+      <c r="E25" t="s">
+        <v>112</v>
+      </c>
+      <c r="F25" s="8">
+        <v>0</v>
+      </c>
+      <c r="G25" s="8">
+        <v>0</v>
+      </c>
+      <c r="H25" s="8">
+        <v>1</v>
+      </c>
+      <c r="I25" s="8">
+        <v>0</v>
+      </c>
+      <c r="J25" t="s">
+        <v>22</v>
+      </c>
+      <c r="K25" s="8">
+        <v>170</v>
+      </c>
+      <c r="L25" s="8">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15">
+      <c r="A26" t="s">
+        <v>113</v>
+      </c>
+      <c r="B26" s="8">
+        <v>1</v>
+      </c>
+      <c r="C26" s="7">
+        <v>4.16</v>
+      </c>
+      <c r="D26" s="7">
+        <v>0.2</v>
+      </c>
+      <c r="E26" t="s">
+        <v>112</v>
+      </c>
+      <c r="F26" s="8">
+        <v>1</v>
+      </c>
+      <c r="G26" s="8">
+        <v>0</v>
+      </c>
+      <c r="H26" s="8">
+        <v>0</v>
+      </c>
+      <c r="I26" s="8">
+        <v>0</v>
+      </c>
+      <c r="J26" t="s">
+        <v>32</v>
+      </c>
+      <c r="K26" s="8">
+        <v>128</v>
+      </c>
+      <c r="L26" s="8">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15">
+      <c r="A27" t="s">
+        <v>114</v>
+      </c>
+      <c r="B27" s="8">
+        <v>1</v>
+      </c>
+      <c r="C27" s="7">
+        <v>4.16</v>
+      </c>
+      <c r="D27" s="7">
+        <v>0.2</v>
+      </c>
+      <c r="E27" t="s">
+        <v>112</v>
+      </c>
+      <c r="F27" s="8">
+        <v>0</v>
+      </c>
+      <c r="G27" s="8">
+        <v>1</v>
+      </c>
+      <c r="H27" s="8">
+        <v>0</v>
+      </c>
+      <c r="I27" s="8">
+        <v>0</v>
+      </c>
+      <c r="J27" t="s">
+        <v>12</v>
+      </c>
+      <c r="K27" s="8">
+        <v>170</v>
+      </c>
+      <c r="L27" s="8">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15">
+      <c r="A28" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15">
+      <c r="A30" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="B30" s="2"/>
+      <c r="C30" s="2"/>
+      <c r="D30" s="2"/>
+      <c r="E30" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15">
+      <c r="A31" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="B31" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="C31" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="D31" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="E31" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="F31" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="G31" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="H31" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="I31" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="J31" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="K31" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="L31" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="M31" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="N31" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="O31" s="6" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15">
+      <c r="A32" t="s">
+        <v>121</v>
+      </c>
+      <c r="B32" s="8">
+        <v>1</v>
+      </c>
+      <c r="C32" s="7">
+        <v>4.16</v>
+      </c>
+      <c r="D32" s="7">
+        <v>0.2</v>
+      </c>
+      <c r="E32" t="s">
+        <v>112</v>
+      </c>
+      <c r="F32" s="8">
+        <v>0</v>
+      </c>
+      <c r="G32" s="8">
+        <v>1</v>
+      </c>
+      <c r="H32" s="8">
+        <v>0</v>
+      </c>
+      <c r="I32" s="8">
+        <v>0</v>
+      </c>
+      <c r="J32" t="s">
+        <v>44</v>
+      </c>
+      <c r="K32" t="s">
+        <v>46</v>
+      </c>
+      <c r="L32" s="8">
+        <v>0</v>
+      </c>
+      <c r="M32" s="8">
+        <v>0</v>
+      </c>
+      <c r="N32" s="8">
+        <v>170</v>
+      </c>
+      <c r="O32" s="8">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="33" spans="1:18">
+      <c r="A33" t="s">
+        <v>122</v>
+      </c>
+      <c r="B33" s="8">
+        <v>1</v>
+      </c>
+      <c r="C33" s="7">
+        <v>4.16</v>
+      </c>
+      <c r="D33" s="7">
+        <v>0.2</v>
+      </c>
+      <c r="E33" t="s">
+        <v>112</v>
+      </c>
+      <c r="F33" s="8">
+        <v>1</v>
+      </c>
+      <c r="G33" s="8">
+        <v>0</v>
+      </c>
+      <c r="H33" s="8">
+        <v>0</v>
+      </c>
+      <c r="I33" s="8">
+        <v>0</v>
+      </c>
+      <c r="J33" t="s">
+        <v>24</v>
+      </c>
+      <c r="K33" t="s">
+        <v>25</v>
+      </c>
+      <c r="L33" s="8">
+        <v>230</v>
+      </c>
+      <c r="M33" s="8">
+        <v>132</v>
+      </c>
+      <c r="N33" s="8">
+        <v>0</v>
+      </c>
+      <c r="O33" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:18">
+      <c r="A34" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="36" spans="1:18">
+      <c r="A36" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="B36" s="2"/>
+      <c r="C36" s="2"/>
+      <c r="D36" s="2"/>
+      <c r="E36" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="37" spans="1:18">
+      <c r="A37" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="B37" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="C37" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="D37" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="E37" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="F37" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="G37" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="H37" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="I37" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="J37" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="K37" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="L37" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="M37" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="N37" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="O37" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="P37" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="Q37" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="R37" s="6" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="38" spans="1:18">
+      <c r="A38" t="s">
+        <v>127</v>
+      </c>
+      <c r="B38" s="8">
+        <v>1</v>
+      </c>
+      <c r="C38" s="7">
+        <v>4.16</v>
+      </c>
+      <c r="D38" s="7">
+        <v>0.2</v>
+      </c>
+      <c r="E38" t="s">
+        <v>112</v>
+      </c>
+      <c r="F38" s="8">
+        <v>0</v>
+      </c>
+      <c r="G38" s="8">
+        <v>0</v>
+      </c>
+      <c r="H38" s="8">
+        <v>1</v>
+      </c>
+      <c r="I38" s="8">
+        <v>0</v>
+      </c>
+      <c r="J38" t="s">
+        <v>36</v>
+      </c>
+      <c r="K38" t="s">
+        <v>37</v>
+      </c>
+      <c r="L38" t="s">
+        <v>38</v>
+      </c>
+      <c r="M38" s="8">
+        <v>485</v>
+      </c>
+      <c r="N38" s="8">
+        <v>190</v>
+      </c>
+      <c r="O38" s="8">
+        <v>68</v>
+      </c>
+      <c r="P38" s="8">
         <v>60</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>51</v>
-      </c>
-      <c r="B6" t="s">
-        <v>61</v>
-      </c>
-      <c r="C6" t="s">
-        <v>63</v>
-      </c>
-      <c r="D6" t="s">
-        <v>65</v>
-      </c>
-      <c r="E6" t="s">
-        <v>68</v>
-      </c>
-      <c r="F6" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>55</v>
-      </c>
-      <c r="B9" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>51</v>
-      </c>
-      <c r="B10" t="s">
-        <v>61</v>
-      </c>
-      <c r="C10" t="s">
-        <v>64</v>
-      </c>
-      <c r="D10" t="s">
-        <v>66</v>
-      </c>
-      <c r="E10" t="s">
-        <v>69</v>
-      </c>
-      <c r="F10" t="s">
-        <v>72</v>
-      </c>
-      <c r="G10" t="s">
-        <v>73</v>
-      </c>
-      <c r="H10" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>56</v>
-      </c>
-      <c r="B11" t="s">
-        <v>26</v>
-      </c>
-      <c r="C11" t="s">
-        <v>27</v>
-      </c>
-      <c r="D11" t="s">
-        <v>28</v>
-      </c>
-      <c r="E11">
+      <c r="Q38" s="8">
+        <v>290</v>
+      </c>
+      <c r="R38" s="8">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="39" spans="1:18">
+      <c r="A39" t="s">
+        <v>128</v>
+      </c>
+      <c r="B39" s="8">
+        <v>1</v>
+      </c>
+      <c r="C39" s="7">
+        <v>0.48</v>
+      </c>
+      <c r="D39" s="7">
+        <v>0.2</v>
+      </c>
+      <c r="E39" t="s">
+        <v>112</v>
+      </c>
+      <c r="F39" s="8">
+        <v>0</v>
+      </c>
+      <c r="G39" s="8">
+        <v>0</v>
+      </c>
+      <c r="H39" s="8">
+        <v>1</v>
+      </c>
+      <c r="I39" s="8">
+        <v>0</v>
+      </c>
+      <c r="J39" t="s">
+        <v>19</v>
+      </c>
+      <c r="K39" t="s">
+        <v>20</v>
+      </c>
+      <c r="L39" t="s">
+        <v>21</v>
+      </c>
+      <c r="M39" s="8">
+        <v>160</v>
+      </c>
+      <c r="N39" s="8">
+        <v>110</v>
+      </c>
+      <c r="O39" s="8">
+        <v>120</v>
+      </c>
+      <c r="P39" s="8">
+        <v>90</v>
+      </c>
+      <c r="Q39" s="8">
+        <v>120</v>
+      </c>
+      <c r="R39" s="8">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="40" spans="1:18">
+      <c r="A40" t="s">
+        <v>129</v>
+      </c>
+      <c r="B40" s="8">
+        <v>1</v>
+      </c>
+      <c r="C40" s="7">
         <v>4.16</v>
       </c>
-      <c r="F11">
-        <v>0</v>
-      </c>
-      <c r="G11">
-        <v>200000</v>
-      </c>
-      <c r="H11">
-        <v>200000</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>58</v>
-      </c>
-      <c r="B14" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>51</v>
-      </c>
-      <c r="B15" t="s">
-        <v>61</v>
-      </c>
-      <c r="C15" t="s">
-        <v>64</v>
-      </c>
-      <c r="D15" t="s">
-        <v>66</v>
-      </c>
-      <c r="E15" t="s">
-        <v>69</v>
-      </c>
-      <c r="F15" t="s">
-        <v>72</v>
-      </c>
-      <c r="G15" t="s">
-        <v>74</v>
-      </c>
-      <c r="H15" t="s">
-        <v>76</v>
-      </c>
-      <c r="I15" t="s">
-        <v>77</v>
-      </c>
-      <c r="J15" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>59</v>
+      <c r="D40" s="7">
+        <v>0.2</v>
+      </c>
+      <c r="E40" t="s">
+        <v>112</v>
+      </c>
+      <c r="F40" s="8">
+        <v>0</v>
+      </c>
+      <c r="G40" s="8">
+        <v>0</v>
+      </c>
+      <c r="H40" s="8">
+        <v>1</v>
+      </c>
+      <c r="I40" s="8">
+        <v>0</v>
+      </c>
+      <c r="J40" t="s">
+        <v>33</v>
+      </c>
+      <c r="K40" t="s">
+        <v>34</v>
+      </c>
+      <c r="L40" t="s">
+        <v>35</v>
+      </c>
+      <c r="M40" s="8">
+        <v>385</v>
+      </c>
+      <c r="N40" s="8">
+        <v>220</v>
+      </c>
+      <c r="O40" s="8">
+        <v>385</v>
+      </c>
+      <c r="P40" s="8">
+        <v>220</v>
+      </c>
+      <c r="Q40" s="8">
+        <v>385</v>
+      </c>
+      <c r="R40" s="8">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="41" spans="1:18">
+      <c r="A41" t="s">
+        <v>130</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="15">
+    <mergeCell ref="A8:H8"/>
+    <mergeCell ref="A9:H9"/>
+    <mergeCell ref="A10:H10"/>
+    <mergeCell ref="A11:D11"/>
+    <mergeCell ref="A13:D13"/>
+    <mergeCell ref="A15:D15"/>
+    <mergeCell ref="A17:D17"/>
+    <mergeCell ref="A19:D19"/>
+    <mergeCell ref="A21:D21"/>
+    <mergeCell ref="A23:D23"/>
+    <mergeCell ref="A28:D28"/>
+    <mergeCell ref="A30:D30"/>
+    <mergeCell ref="A34:D34"/>
+    <mergeCell ref="A36:D36"/>
+    <mergeCell ref="A41:D41"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="A2" location="'Load'!A12:E13" display="PositiveSeqZload"/>
+    <hyperlink ref="B2" location="'Load'!A37:R41" display="ThreePhaseZIPLoad"/>
+    <hyperlink ref="A3" location="'Load'!A16:E17" display="PositiveSeqPload"/>
+    <hyperlink ref="A4" location="'Load'!A20:E21" display="PositiveSeqIload"/>
+    <hyperlink ref="A5" location="'Load'!A24:L28" display="SinglePhaseZIPLoad"/>
+    <hyperlink ref="A6" location="'Load'!A31:O34" display="TwoPhaseZIPLoad"/>
+    <hyperlink ref="E11" location="'Load'!A1" display="Go to Type List"/>
+    <hyperlink ref="E15" location="'Load'!A1" display="Go to Type List"/>
+    <hyperlink ref="E19" location="'Load'!A1" display="Go to Type List"/>
+    <hyperlink ref="E23" location="'Load'!A1" display="Go to Type List"/>
+    <hyperlink ref="E30" location="'Load'!A1" display="Go to Type List"/>
+    <hyperlink ref="E36" location="'Load'!A1" display="Go to Type List"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Bug fixes - Now works with 4 bus example
</commit_message>
<xml_diff>
--- a/Outputs/CYME_Extract_13Bus.xlsx
+++ b/Outputs/CYME_Extract_13Bus.xlsx
@@ -762,18 +762,18 @@
     <t>Q1 (kVAr)</t>
   </si>
   <si>
+    <t>LD_652</t>
+  </si>
+  <si>
+    <t>wye</t>
+  </si>
+  <si>
+    <t>LD_611</t>
+  </si>
+  <si>
     <t>LD_645</t>
   </si>
   <si>
-    <t>wye</t>
-  </si>
-  <si>
-    <t>LD_652</t>
-  </si>
-  <si>
-    <t>LD_611</t>
-  </si>
-  <si>
     <t>End of SinglePhase ZIP Load</t>
   </si>
   <si>
@@ -792,12 +792,12 @@
     <t>Q2 (kVAr)</t>
   </si>
   <si>
+    <t>LD_646</t>
+  </si>
+  <si>
     <t>LD_692</t>
   </si>
   <si>
-    <t>LD_646</t>
-  </si>
-  <si>
     <t>End of TwoPhase ZIP Load</t>
   </si>
   <si>
@@ -810,15 +810,15 @@
     <t>Q3 (kVAr)</t>
   </si>
   <si>
+    <t>LD_671</t>
+  </si>
+  <si>
     <t>LD_675</t>
   </si>
   <si>
     <t>LD_634</t>
   </si>
   <si>
-    <t>LD_671</t>
-  </si>
-  <si>
     <t>End of Three-Phase ZIP Load</t>
   </si>
   <si>
@@ -879,12 +879,12 @@
     <t>b11 (uS/length_unit)</t>
   </si>
   <si>
+    <t>LN_684_611</t>
+  </si>
+  <si>
     <t>LN_684_652</t>
   </si>
   <si>
-    <t>LN_684_611</t>
-  </si>
-  <si>
     <t>End of Single-Phase Line</t>
   </si>
   <si>
@@ -915,15 +915,15 @@
     <t>b22 (uS/length_unit)</t>
   </si>
   <si>
+    <t>LN_632_645</t>
+  </si>
+  <si>
+    <t>LN_645_646</t>
+  </si>
+  <si>
     <t>LN_671_684</t>
   </si>
   <si>
-    <t>LN_632_645</t>
-  </si>
-  <si>
-    <t>LN_645_646</t>
-  </si>
-  <si>
     <t>End of Two-Phase Line</t>
   </si>
   <si>
@@ -966,16 +966,16 @@
     <t>LN_651_632</t>
   </si>
   <si>
+    <t>LN_632_671</t>
+  </si>
+  <si>
+    <t>LN_632_633</t>
+  </si>
+  <si>
+    <t>LN_692_675</t>
+  </si>
+  <si>
     <t>LN_671_680</t>
-  </si>
-  <si>
-    <t>LN_632_633</t>
-  </si>
-  <si>
-    <t>LN_692_675</t>
-  </si>
-  <si>
-    <t>LN_632_671</t>
   </si>
   <si>
     <t>End of Three-Phase Line with Full Data</t>
@@ -1644,7 +1644,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="2">
-        <v>67</v>
+        <v>60</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -1652,7 +1652,7 @@
         <v>5</v>
       </c>
       <c r="B4" s="2">
-        <v>117</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -2219,8 +2219,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="2" width="18.7109375" customWidth="1"/>
-    <col min="3" max="3" width="16.7109375" customWidth="1"/>
+    <col min="1" max="3" width="18.7109375" customWidth="1"/>
     <col min="4" max="4" width="8.7109375" customWidth="1"/>
     <col min="5" max="6" width="10.7109375" customWidth="1"/>
   </cols>
@@ -3487,25 +3486,25 @@
         <v>247</v>
       </c>
       <c r="F25" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G25" s="3">
         <v>0</v>
       </c>
       <c r="H25" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I25" s="3">
         <v>0</v>
       </c>
       <c r="J25" t="s">
-        <v>159</v>
+        <v>170</v>
       </c>
       <c r="K25" s="3">
-        <v>170</v>
+        <v>128</v>
       </c>
       <c r="L25" s="3">
-        <v>125</v>
+        <v>86</v>
       </c>
     </row>
     <row r="26" spans="1:15">
@@ -3525,10 +3524,10 @@
         <v>247</v>
       </c>
       <c r="F26" s="3">
+        <v>0</v>
+      </c>
+      <c r="G26" s="3">
         <v>1</v>
-      </c>
-      <c r="G26" s="3">
-        <v>0</v>
       </c>
       <c r="H26" s="3">
         <v>0</v>
@@ -3537,13 +3536,13 @@
         <v>0</v>
       </c>
       <c r="J26" t="s">
+        <v>147</v>
+      </c>
+      <c r="K26" s="3">
         <v>170</v>
       </c>
-      <c r="K26" s="3">
-        <v>128</v>
-      </c>
       <c r="L26" s="3">
-        <v>86</v>
+        <v>80</v>
       </c>
     </row>
     <row r="27" spans="1:15">
@@ -3566,22 +3565,22 @@
         <v>0</v>
       </c>
       <c r="G27" s="3">
+        <v>0</v>
+      </c>
+      <c r="H27" s="3">
         <v>1</v>
-      </c>
-      <c r="H27" s="3">
-        <v>0</v>
       </c>
       <c r="I27" s="3">
         <v>0</v>
       </c>
       <c r="J27" t="s">
-        <v>147</v>
+        <v>159</v>
       </c>
       <c r="K27" s="3">
         <v>170</v>
       </c>
       <c r="L27" s="3">
-        <v>80</v>
+        <v>125</v>
       </c>
     </row>
     <row r="28" spans="1:15">
@@ -3662,10 +3661,10 @@
         <v>247</v>
       </c>
       <c r="F32" s="3">
+        <v>1</v>
+      </c>
+      <c r="G32" s="3">
         <v>0</v>
-      </c>
-      <c r="G32" s="3">
-        <v>1</v>
       </c>
       <c r="H32" s="3">
         <v>0</v>
@@ -3674,22 +3673,22 @@
         <v>0</v>
       </c>
       <c r="J32" t="s">
-        <v>182</v>
+        <v>161</v>
       </c>
       <c r="K32" t="s">
-        <v>184</v>
+        <v>162</v>
       </c>
       <c r="L32" s="3">
+        <v>230</v>
+      </c>
+      <c r="M32" s="3">
+        <v>132</v>
+      </c>
+      <c r="N32" s="3">
         <v>0</v>
       </c>
-      <c r="M32" s="3">
+      <c r="O32" s="3">
         <v>0</v>
-      </c>
-      <c r="N32" s="3">
-        <v>170</v>
-      </c>
-      <c r="O32" s="3">
-        <v>151</v>
       </c>
     </row>
     <row r="33" spans="1:18">
@@ -3709,10 +3708,10 @@
         <v>247</v>
       </c>
       <c r="F33" s="3">
+        <v>0</v>
+      </c>
+      <c r="G33" s="3">
         <v>1</v>
-      </c>
-      <c r="G33" s="3">
-        <v>0</v>
       </c>
       <c r="H33" s="3">
         <v>0</v>
@@ -3721,22 +3720,22 @@
         <v>0</v>
       </c>
       <c r="J33" t="s">
-        <v>161</v>
+        <v>182</v>
       </c>
       <c r="K33" t="s">
-        <v>162</v>
+        <v>184</v>
       </c>
       <c r="L33" s="3">
-        <v>230</v>
+        <v>0</v>
       </c>
       <c r="M33" s="3">
-        <v>132</v>
+        <v>0</v>
       </c>
       <c r="N33" s="3">
-        <v>0</v>
+        <v>170</v>
       </c>
       <c r="O33" s="3">
-        <v>0</v>
+        <v>151</v>
       </c>
     </row>
     <row r="34" spans="1:18">
@@ -3838,31 +3837,31 @@
         <v>0</v>
       </c>
       <c r="J38" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="K38" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="L38" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="M38" s="3">
-        <v>485</v>
+        <v>385</v>
       </c>
       <c r="N38" s="3">
-        <v>190</v>
+        <v>220</v>
       </c>
       <c r="O38" s="3">
-        <v>68</v>
+        <v>385</v>
       </c>
       <c r="P38" s="3">
-        <v>60</v>
+        <v>220</v>
       </c>
       <c r="Q38" s="3">
-        <v>290</v>
+        <v>385</v>
       </c>
       <c r="R38" s="3">
-        <v>212</v>
+        <v>220</v>
       </c>
     </row>
     <row r="39" spans="1:18">
@@ -3873,7 +3872,7 @@
         <v>1</v>
       </c>
       <c r="C39" s="2">
-        <v>0.48</v>
+        <v>4.16</v>
       </c>
       <c r="D39" s="2">
         <v>0.2</v>
@@ -3894,31 +3893,31 @@
         <v>0</v>
       </c>
       <c r="J39" t="s">
-        <v>156</v>
+        <v>174</v>
       </c>
       <c r="K39" t="s">
-        <v>157</v>
+        <v>175</v>
       </c>
       <c r="L39" t="s">
-        <v>158</v>
+        <v>176</v>
       </c>
       <c r="M39" s="3">
-        <v>160</v>
+        <v>485</v>
       </c>
       <c r="N39" s="3">
-        <v>110</v>
+        <v>190</v>
       </c>
       <c r="O39" s="3">
-        <v>120</v>
+        <v>68</v>
       </c>
       <c r="P39" s="3">
-        <v>90</v>
+        <v>60</v>
       </c>
       <c r="Q39" s="3">
-        <v>120</v>
+        <v>290</v>
       </c>
       <c r="R39" s="3">
-        <v>90</v>
+        <v>212</v>
       </c>
     </row>
     <row r="40" spans="1:18">
@@ -3929,7 +3928,7 @@
         <v>1</v>
       </c>
       <c r="C40" s="2">
-        <v>4.16</v>
+        <v>0.48</v>
       </c>
       <c r="D40" s="2">
         <v>0.2</v>
@@ -3950,31 +3949,31 @@
         <v>0</v>
       </c>
       <c r="J40" t="s">
-        <v>171</v>
+        <v>156</v>
       </c>
       <c r="K40" t="s">
-        <v>172</v>
+        <v>157</v>
       </c>
       <c r="L40" t="s">
-        <v>173</v>
+        <v>158</v>
       </c>
       <c r="M40" s="3">
-        <v>385</v>
+        <v>160</v>
       </c>
       <c r="N40" s="3">
-        <v>220</v>
+        <v>110</v>
       </c>
       <c r="O40" s="3">
-        <v>385</v>
+        <v>120</v>
       </c>
       <c r="P40" s="3">
-        <v>220</v>
+        <v>90</v>
       </c>
       <c r="Q40" s="3">
-        <v>385</v>
+        <v>120</v>
       </c>
       <c r="R40" s="3">
-        <v>220</v>
+        <v>90</v>
       </c>
     </row>
     <row r="41" spans="1:18">
@@ -4179,22 +4178,22 @@
         <v>1</v>
       </c>
       <c r="C17" s="8">
-        <v>0.15151515145728</v>
+        <v>0.05681818303922239</v>
       </c>
       <c r="D17" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="E17" t="s">
-        <v>170</v>
+        <v>147</v>
       </c>
       <c r="F17" s="9">
-        <v>0.5183422560256721</v>
+        <v>0.5111219227746321</v>
       </c>
       <c r="G17" s="9">
-        <v>0.19783837382088</v>
+        <v>0.5239016640804961</v>
       </c>
       <c r="H17" s="9">
-        <v>34.35968505110118</v>
+        <v>1.801475010248056</v>
       </c>
     </row>
     <row r="18" spans="1:27">
@@ -4205,22 +4204,22 @@
         <v>1</v>
       </c>
       <c r="C18" s="8">
-        <v>0.05681818303922239</v>
+        <v>0.15151515145728</v>
       </c>
       <c r="D18" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="E18" t="s">
-        <v>147</v>
+        <v>170</v>
       </c>
       <c r="F18" s="9">
-        <v>0.5111219227746321</v>
+        <v>0.5183422560256721</v>
       </c>
       <c r="G18" s="9">
-        <v>0.5239016640804961</v>
+        <v>0.19783837382088</v>
       </c>
       <c r="H18" s="9">
-        <v>1.801475010248056</v>
+        <v>34.35968505110118</v>
       </c>
     </row>
     <row r="19" spans="1:27">
@@ -4295,31 +4294,31 @@
         <v>1</v>
       </c>
       <c r="C23" s="8">
-        <v>0.05681818179648</v>
+        <v>0.0946969696608</v>
       </c>
       <c r="D23" t="s">
-        <v>171</v>
+        <v>151</v>
       </c>
       <c r="E23" t="s">
-        <v>173</v>
+        <v>152</v>
       </c>
       <c r="F23" t="s">
-        <v>180</v>
+        <v>159</v>
       </c>
       <c r="G23" t="s">
-        <v>181</v>
+        <v>160</v>
       </c>
       <c r="H23" s="9">
-        <v>0</v>
+        <v>0.513284294522792</v>
       </c>
       <c r="I23" s="9">
-        <v>0</v>
+        <v>0.520118134892408</v>
       </c>
       <c r="J23" s="9">
-        <v>0</v>
+        <v>0.07976914814419199</v>
       </c>
       <c r="K23" s="9">
-        <v>0</v>
+        <v>0.177259802684224</v>
       </c>
       <c r="L23" s="9">
         <v>0.5111219227746321</v>
@@ -4328,10 +4327,10 @@
         <v>0.5239016640804961</v>
       </c>
       <c r="N23" s="9">
-        <v>0</v>
+        <v>1.818424773623432</v>
       </c>
       <c r="O23" s="9">
-        <v>0</v>
+        <v>-0.347453372173024</v>
       </c>
       <c r="P23" s="9">
         <v>1.801475010248056</v>
@@ -4345,19 +4344,19 @@
         <v>1</v>
       </c>
       <c r="C24" s="8">
-        <v>0.0946969696608</v>
+        <v>0.05681818179648</v>
       </c>
       <c r="D24" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="E24" t="s">
-        <v>152</v>
+        <v>160</v>
       </c>
       <c r="F24" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="G24" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="H24" s="9">
         <v>0.513284294522792</v>
@@ -4398,28 +4397,28 @@
         <v>0.05681818179648</v>
       </c>
       <c r="D25" t="s">
-        <v>159</v>
+        <v>171</v>
       </c>
       <c r="E25" t="s">
-        <v>160</v>
+        <v>173</v>
       </c>
       <c r="F25" t="s">
-        <v>161</v>
+        <v>180</v>
       </c>
       <c r="G25" t="s">
-        <v>162</v>
+        <v>181</v>
       </c>
       <c r="H25" s="9">
-        <v>0.513284294522792</v>
+        <v>0</v>
       </c>
       <c r="I25" s="9">
-        <v>0.520118134892408</v>
+        <v>0</v>
       </c>
       <c r="J25" s="9">
-        <v>0.07976914814419199</v>
+        <v>0</v>
       </c>
       <c r="K25" s="9">
-        <v>0.177259802684224</v>
+        <v>0</v>
       </c>
       <c r="L25" s="9">
         <v>0.5111219227746321</v>
@@ -4428,10 +4427,10 @@
         <v>0.5239016640804961</v>
       </c>
       <c r="N25" s="9">
-        <v>1.818424773623432</v>
+        <v>0</v>
       </c>
       <c r="O25" s="9">
-        <v>-0.347453372173024</v>
+        <v>0</v>
       </c>
       <c r="P25" s="9">
         <v>1.801475010248056</v>
@@ -4625,25 +4624,25 @@
         <v>1</v>
       </c>
       <c r="C31" s="8">
-        <v>0.1893939393216</v>
+        <v>0.3787880029174384</v>
       </c>
       <c r="D31" t="s">
+        <v>150</v>
+      </c>
+      <c r="E31" t="s">
+        <v>151</v>
+      </c>
+      <c r="F31" t="s">
+        <v>152</v>
+      </c>
+      <c r="G31" t="s">
         <v>171</v>
       </c>
-      <c r="E31" t="s">
+      <c r="H31" t="s">
         <v>172</v>
       </c>
-      <c r="F31" t="s">
+      <c r="I31" t="s">
         <v>173</v>
-      </c>
-      <c r="G31" t="s">
-        <v>177</v>
-      </c>
-      <c r="H31" t="s">
-        <v>178</v>
-      </c>
-      <c r="I31" t="s">
-        <v>179</v>
       </c>
       <c r="J31" s="9">
         <v>0.13378432449356</v>
@@ -4874,25 +4873,25 @@
         <v>1</v>
       </c>
       <c r="C34" s="8">
-        <v>0.3787880029174384</v>
+        <v>0.1893939393216</v>
       </c>
       <c r="D34" t="s">
-        <v>150</v>
+        <v>171</v>
       </c>
       <c r="E34" t="s">
-        <v>151</v>
+        <v>172</v>
       </c>
       <c r="F34" t="s">
-        <v>152</v>
+        <v>173</v>
       </c>
       <c r="G34" t="s">
-        <v>171</v>
+        <v>177</v>
       </c>
       <c r="H34" t="s">
-        <v>172</v>
+        <v>178</v>
       </c>
       <c r="I34" t="s">
-        <v>173</v>
+        <v>179</v>
       </c>
       <c r="J34" s="9">
         <v>0.13378432449356</v>

</xml_diff>

<commit_message>
Fixed bus and voltage source
</commit_message>
<xml_diff>
--- a/Outputs/CYME_Extract_13Bus.xlsx
+++ b/Outputs/CYME_Extract_13Bus.xlsx
@@ -579,6 +579,15 @@
     <t>692_c</t>
   </si>
   <si>
+    <t>Important notes:</t>
+  </si>
+  <si>
+    <t>Default order of blocks and columns after row 11 must not change</t>
+  </si>
+  <si>
+    <t>One empty row between End of each block and the next block is mandatory; otherwise, empty rows are NOT allowed</t>
+  </si>
+  <si>
     <t>PositiveSeqVsource</t>
   </si>
   <si>
@@ -591,15 +600,6 @@
     <t>ThreePhaseSequentialVsource</t>
   </si>
   <si>
-    <t>Important notes:</t>
-  </si>
-  <si>
-    <t>Default order of blocks and columns after row 11 must not change</t>
-  </si>
-  <si>
-    <t>One empty row between End of each block and the next block is mandatory; otherwise, empty rows are NOT allowed</t>
-  </si>
-  <si>
     <t>Positive-Sequence Voltage Source</t>
   </si>
   <si>
@@ -663,27 +663,27 @@
     <t>SC3ph (MVA)</t>
   </si>
   <si>
+    <t>End of Three-Phase Voltage Source with Short-Circuit Level Data</t>
+  </si>
+  <si>
+    <t>Three-Phase Voltage Source with Sequential Data</t>
+  </si>
+  <si>
+    <t>R1 (Ohm)</t>
+  </si>
+  <si>
+    <t>X1 (Ohm)</t>
+  </si>
+  <si>
+    <t>R0 (Ohm)</t>
+  </si>
+  <si>
+    <t>X0 (Ohm)</t>
+  </si>
+  <si>
     <t>SUB650WYE</t>
   </si>
   <si>
-    <t>End of Three-Phase Voltage Source with Short-Circuit Level Data</t>
-  </si>
-  <si>
-    <t>Three-Phase Voltage Source with Sequential Data</t>
-  </si>
-  <si>
-    <t>R1 (Ohm)</t>
-  </si>
-  <si>
-    <t>X1 (Ohm)</t>
-  </si>
-  <si>
-    <t>R0 (Ohm)</t>
-  </si>
-  <si>
-    <t>X0 (Ohm)</t>
-  </si>
-  <si>
     <t>End of Three-Phase Voltage Source with Sequential Data</t>
   </si>
   <si>
@@ -762,16 +762,16 @@
     <t>Q1 (kVAr)</t>
   </si>
   <si>
-    <t>LD_652</t>
+    <t>LD_LOAD652</t>
   </si>
   <si>
     <t>wye</t>
   </si>
   <si>
-    <t>LD_611</t>
-  </si>
-  <si>
-    <t>LD_645</t>
+    <t>LD_LOAD611</t>
+  </si>
+  <si>
+    <t>LD_LOAD645</t>
   </si>
   <si>
     <t>End of SinglePhase ZIP Load</t>
@@ -792,10 +792,10 @@
     <t>Q2 (kVAr)</t>
   </si>
   <si>
-    <t>LD_646</t>
-  </si>
-  <si>
-    <t>LD_692</t>
+    <t>LD_LOAD646</t>
+  </si>
+  <si>
+    <t>LD_LOAD692</t>
   </si>
   <si>
     <t>End of TwoPhase ZIP Load</t>
@@ -810,13 +810,13 @@
     <t>Q3 (kVAr)</t>
   </si>
   <si>
-    <t>LD_671</t>
-  </si>
-  <si>
-    <t>LD_675</t>
-  </si>
-  <si>
-    <t>LD_634</t>
+    <t>LD_LOAD671</t>
+  </si>
+  <si>
+    <t>LD_LOAD675</t>
+  </si>
+  <si>
+    <t>LD_LOAD634</t>
   </si>
   <si>
     <t>End of Three-Phase ZIP Load</t>
@@ -2972,27 +2972,27 @@
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="4" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="4" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="4" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" s="4" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" s="5" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>
@@ -3004,7 +3004,7 @@
     </row>
     <row r="9" spans="1:8">
       <c r="A9" s="6" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
@@ -3016,7 +3016,7 @@
     </row>
     <row r="10" spans="1:8">
       <c r="A10" s="6" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
@@ -3139,74 +3139,77 @@
       <c r="A21" t="s">
         <v>213</v>
       </c>
-      <c r="B21" t="s">
+    </row>
+    <row r="23" spans="1:10">
+      <c r="A23" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="4" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10">
+      <c r="A24" s="7" t="s">
+        <v>194</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>201</v>
+      </c>
+      <c r="C24" s="7" t="s">
+        <v>207</v>
+      </c>
+      <c r="D24" s="7" t="s">
+        <v>208</v>
+      </c>
+      <c r="E24" s="7" t="s">
+        <v>209</v>
+      </c>
+      <c r="F24" s="7" t="s">
+        <v>210</v>
+      </c>
+      <c r="G24" s="7" t="s">
+        <v>215</v>
+      </c>
+      <c r="H24" s="7" t="s">
+        <v>216</v>
+      </c>
+      <c r="I24" s="7" t="s">
+        <v>217</v>
+      </c>
+      <c r="J24" s="7" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10">
+      <c r="A25" t="s">
+        <v>219</v>
+      </c>
+      <c r="B25" t="s">
         <v>163</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C25" t="s">
         <v>165</v>
       </c>
-      <c r="D21" t="s">
+      <c r="D25" t="s">
         <v>166</v>
       </c>
-      <c r="E21" s="2">
+      <c r="E25" s="2">
         <v>4.16</v>
       </c>
-      <c r="F21" s="2">
-        <v>0</v>
-      </c>
-      <c r="G21" s="3">
-        <v>200000</v>
-      </c>
-      <c r="H21" s="3">
-        <v>200000</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10">
-      <c r="A22" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10">
-      <c r="A24" s="1" t="s">
-        <v>215</v>
-      </c>
-      <c r="B24" s="1"/>
-      <c r="C24" s="1"/>
-      <c r="D24" s="1"/>
-      <c r="E24" s="4" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10">
-      <c r="A25" s="7" t="s">
-        <v>194</v>
-      </c>
-      <c r="B25" s="7" t="s">
-        <v>201</v>
-      </c>
-      <c r="C25" s="7" t="s">
-        <v>207</v>
-      </c>
-      <c r="D25" s="7" t="s">
-        <v>208</v>
-      </c>
-      <c r="E25" s="7" t="s">
-        <v>209</v>
-      </c>
-      <c r="F25" s="7" t="s">
-        <v>210</v>
-      </c>
-      <c r="G25" s="7" t="s">
-        <v>216</v>
-      </c>
-      <c r="H25" s="7" t="s">
-        <v>217</v>
-      </c>
-      <c r="I25" s="7" t="s">
-        <v>218</v>
-      </c>
-      <c r="J25" s="7" t="s">
-        <v>219</v>
+      <c r="G25" s="2">
+        <v>0.001731</v>
+      </c>
+      <c r="H25" s="2">
+        <v>0.013844</v>
+      </c>
+      <c r="I25" s="2">
+        <v>0.001731</v>
+      </c>
+      <c r="J25" s="2">
+        <v>0.013844</v>
       </c>
     </row>
     <row r="26" spans="1:10">
@@ -3224,19 +3227,19 @@
     <mergeCell ref="A15:D15"/>
     <mergeCell ref="A17:D17"/>
     <mergeCell ref="A19:D19"/>
-    <mergeCell ref="A22:D22"/>
-    <mergeCell ref="A24:D24"/>
+    <mergeCell ref="A21:D21"/>
+    <mergeCell ref="A23:D23"/>
     <mergeCell ref="A26:D26"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A2" location="'Voltage Source'!A12:F13" display="PositiveSeqVsource"/>
     <hyperlink ref="A3" location="'Voltage Source'!A16:F17" display="SinglePhaseVsource"/>
-    <hyperlink ref="A4" location="'Voltage Source'!A20:H22" display="ThreePhaseShortCircuitVsource"/>
-    <hyperlink ref="A5" location="'Voltage Source'!A25:J26" display="ThreePhaseSequentialVsource"/>
+    <hyperlink ref="A4" location="'Voltage Source'!A20:H21" display="ThreePhaseShortCircuitVsource"/>
+    <hyperlink ref="A5" location="'Voltage Source'!A24:J26" display="ThreePhaseSequentialVsource"/>
     <hyperlink ref="E11" location="'Voltage Source'!A1" display="Go to Type List"/>
     <hyperlink ref="E15" location="'Voltage Source'!A1" display="Go to Type List"/>
     <hyperlink ref="E19" location="'Voltage Source'!A1" display="Go to Type List"/>
-    <hyperlink ref="E24" location="'Voltage Source'!A1" display="Go to Type List"/>
+    <hyperlink ref="E23" location="'Voltage Source'!A1" display="Go to Type List"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3295,7 +3298,7 @@
     </row>
     <row r="8" spans="1:8">
       <c r="A8" s="5" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>
@@ -3307,7 +3310,7 @@
     </row>
     <row r="9" spans="1:8">
       <c r="A9" s="6" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
@@ -3319,7 +3322,7 @@
     </row>
     <row r="10" spans="1:8">
       <c r="A10" s="6" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
@@ -4064,7 +4067,7 @@
     </row>
     <row r="8" spans="1:8">
       <c r="A8" s="5" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>
@@ -4076,7 +4079,7 @@
     </row>
     <row r="9" spans="1:8">
       <c r="A9" s="6" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
@@ -4088,7 +4091,7 @@
     </row>
     <row r="10" spans="1:8">
       <c r="A10" s="6" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
@@ -5100,7 +5103,7 @@
     </row>
     <row r="8" spans="1:19">
       <c r="A8" s="5" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>
@@ -5112,7 +5115,7 @@
     </row>
     <row r="9" spans="1:19">
       <c r="A9" s="6" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
@@ -5124,7 +5127,7 @@
     </row>
     <row r="10" spans="1:19">
       <c r="A10" s="6" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
@@ -5593,7 +5596,7 @@
     </row>
     <row r="8" spans="1:8">
       <c r="A8" s="5" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>
@@ -5605,7 +5608,7 @@
     </row>
     <row r="9" spans="1:8">
       <c r="A9" s="6" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
@@ -5617,7 +5620,7 @@
     </row>
     <row r="10" spans="1:8">
       <c r="A10" s="6" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>

</xml_diff>

<commit_message>
Does not handle islands. Working when no islands and troublesome switches are removed.
</commit_message>
<xml_diff>
--- a/Outputs/CYME_Extract_13Bus.xlsx
+++ b/Outputs/CYME_Extract_13Bus.xlsx
@@ -14,15 +14,15 @@
     <sheet name="Load" sheetId="5" r:id="rId5"/>
     <sheet name="Line" sheetId="6" r:id="rId6"/>
     <sheet name="Transformer" sheetId="7" r:id="rId7"/>
-    <sheet name="Shunt" sheetId="8" r:id="rId8"/>
-    <sheet name="Switch" sheetId="9" r:id="rId9"/>
+    <sheet name="Switch" sheetId="8" r:id="rId8"/>
+    <sheet name="Shunt" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="809" uniqueCount="398">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="814" uniqueCount="399">
   <si>
     <t>Excel file version</t>
   </si>
@@ -42,7 +42,7 @@
     <t>Power Base (MVA)</t>
   </si>
   <si>
-    <t>outgoing</t>
+    <t>//outgoing</t>
   </si>
   <si>
     <t>V_abs</t>
@@ -432,7 +432,7 @@
     <t>LD_692/Q2</t>
   </si>
   <si>
-    <t>incoming</t>
+    <t>//incoming</t>
   </si>
   <si>
     <t>Trans_tap</t>
@@ -516,7 +516,7 @@
     <t>650_a</t>
   </si>
   <si>
-    <t>Slack</t>
+    <t>SLACK</t>
   </si>
   <si>
     <t>650_b</t>
@@ -654,7 +654,7 @@
     <t>kV (ph-ph RMS)</t>
   </si>
   <si>
-    <t>Angle_a (deg)</t>
+    <t xml:space="preserve"> Angle_a (deg)</t>
   </si>
   <si>
     <t>SC1ph (MVA)</t>
@@ -681,7 +681,7 @@
     <t>X0 (Ohm)</t>
   </si>
   <si>
-    <t>SUB650WYE</t>
+    <t>SRC_SUB650WYE</t>
   </si>
   <si>
     <t>End of Three-Phase Voltage Source with Sequential Data</t>
@@ -780,7 +780,7 @@
     <t>LD_LOAD692</t>
   </si>
   <si>
-    <t>End of SinglePhase ZIP Load</t>
+    <t>End of Single-Phase ZIP Load</t>
   </si>
   <si>
     <t>Two-Phase ZIP Load</t>
@@ -798,7 +798,7 @@
     <t>Q2 (kVAr)</t>
   </si>
   <si>
-    <t>End of TwoPhase ZIP Load</t>
+    <t>End of Two-Phase ZIP Load</t>
   </si>
   <si>
     <t>Three-Phase ZIP Load</t>
@@ -813,6 +813,9 @@
     <t>LD_LOAD671</t>
   </si>
   <si>
+    <t>LD_L632_671_1</t>
+  </si>
+  <si>
     <t>LD_LOAD675</t>
   </si>
   <si>
@@ -1140,6 +1143,30 @@
     <t>End of Multiphase 2W-Transformer with Mutual Impedance</t>
   </si>
   <si>
+    <t>From Bus</t>
+  </si>
+  <si>
+    <t>To Bus</t>
+  </si>
+  <si>
+    <t>296_a</t>
+  </si>
+  <si>
+    <t>296_b</t>
+  </si>
+  <si>
+    <t>296_c</t>
+  </si>
+  <si>
+    <t>L671_692_SW_1_a</t>
+  </si>
+  <si>
+    <t>L671_692_SW_1_b</t>
+  </si>
+  <si>
+    <t>L671_692_SW_1_c</t>
+  </si>
+  <si>
     <t>PositiveSeqShunt</t>
   </si>
   <si>
@@ -1192,30 +1219,6 @@
   </si>
   <si>
     <t>End of Three-Phase Shunt</t>
-  </si>
-  <si>
-    <t>From Bus</t>
-  </si>
-  <si>
-    <t>To Bus</t>
-  </si>
-  <si>
-    <t>296_a</t>
-  </si>
-  <si>
-    <t>296_b</t>
-  </si>
-  <si>
-    <t>296_c</t>
-  </si>
-  <si>
-    <t>L671_692_SW-1_a</t>
-  </si>
-  <si>
-    <t>L671_692_SW-1_b</t>
-  </si>
-  <si>
-    <t>L671_692_SW-1_c</t>
   </si>
 </sst>
 </file>
@@ -3250,7 +3253,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:R41"/>
+  <dimension ref="A1:R42"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3881,31 +3884,31 @@
         <v>0</v>
       </c>
       <c r="J39" t="s">
-        <v>174</v>
+        <v>150</v>
       </c>
       <c r="K39" t="s">
-        <v>175</v>
+        <v>151</v>
       </c>
       <c r="L39" t="s">
-        <v>176</v>
+        <v>152</v>
       </c>
       <c r="M39" s="3">
-        <v>485</v>
+        <v>17</v>
       </c>
       <c r="N39" s="3">
-        <v>190</v>
+        <v>10</v>
       </c>
       <c r="O39" s="3">
+        <v>66</v>
+      </c>
+      <c r="P39" s="3">
+        <v>38</v>
+      </c>
+      <c r="Q39" s="3">
+        <v>117</v>
+      </c>
+      <c r="R39" s="3">
         <v>68</v>
-      </c>
-      <c r="P39" s="3">
-        <v>60</v>
-      </c>
-      <c r="Q39" s="3">
-        <v>290</v>
-      </c>
-      <c r="R39" s="3">
-        <v>212</v>
       </c>
     </row>
     <row r="40" spans="1:18">
@@ -3916,7 +3919,7 @@
         <v>1</v>
       </c>
       <c r="C40" s="2">
-        <v>0.48</v>
+        <v>4.16</v>
       </c>
       <c r="D40" s="2">
         <v>0.2</v>
@@ -3937,36 +3940,92 @@
         <v>0</v>
       </c>
       <c r="J40" t="s">
-        <v>156</v>
+        <v>174</v>
       </c>
       <c r="K40" t="s">
-        <v>157</v>
+        <v>175</v>
       </c>
       <c r="L40" t="s">
-        <v>158</v>
+        <v>176</v>
       </c>
       <c r="M40" s="3">
-        <v>160</v>
+        <v>485</v>
       </c>
       <c r="N40" s="3">
-        <v>110</v>
+        <v>190</v>
       </c>
       <c r="O40" s="3">
-        <v>120</v>
+        <v>68</v>
       </c>
       <c r="P40" s="3">
-        <v>90</v>
+        <v>60</v>
       </c>
       <c r="Q40" s="3">
-        <v>120</v>
+        <v>290</v>
       </c>
       <c r="R40" s="3">
-        <v>90</v>
+        <v>212</v>
       </c>
     </row>
     <row r="41" spans="1:18">
       <c r="A41" t="s">
         <v>265</v>
+      </c>
+      <c r="B41" s="3">
+        <v>1</v>
+      </c>
+      <c r="C41" s="2">
+        <v>0.48</v>
+      </c>
+      <c r="D41" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="E41" t="s">
+        <v>247</v>
+      </c>
+      <c r="F41" s="3">
+        <v>0</v>
+      </c>
+      <c r="G41" s="3">
+        <v>0</v>
+      </c>
+      <c r="H41" s="3">
+        <v>1</v>
+      </c>
+      <c r="I41" s="3">
+        <v>0</v>
+      </c>
+      <c r="J41" t="s">
+        <v>156</v>
+      </c>
+      <c r="K41" t="s">
+        <v>157</v>
+      </c>
+      <c r="L41" t="s">
+        <v>158</v>
+      </c>
+      <c r="M41" s="3">
+        <v>160</v>
+      </c>
+      <c r="N41" s="3">
+        <v>110</v>
+      </c>
+      <c r="O41" s="3">
+        <v>120</v>
+      </c>
+      <c r="P41" s="3">
+        <v>90</v>
+      </c>
+      <c r="Q41" s="3">
+        <v>120</v>
+      </c>
+      <c r="R41" s="3">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="42" spans="1:18">
+      <c r="A42" t="s">
+        <v>266</v>
       </c>
     </row>
   </sheetData>
@@ -3985,11 +4044,11 @@
     <mergeCell ref="A32:B32"/>
     <mergeCell ref="A34:B34"/>
     <mergeCell ref="A36:B36"/>
-    <mergeCell ref="A41:B41"/>
+    <mergeCell ref="A42:B42"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A2" location="'Load'!A12:E13" display="PositiveSeqZload"/>
-    <hyperlink ref="B2" location="'Load'!A37:R41" display="ThreePhaseZIPLoad"/>
+    <hyperlink ref="B2" location="'Load'!A37:R42" display="ThreePhaseZIPLoad"/>
     <hyperlink ref="A3" location="'Load'!A16:E17" display="PositiveSeqPload"/>
     <hyperlink ref="A4" location="'Load'!A20:E21" display="PositiveSeqIload"/>
     <hyperlink ref="A5" location="'Load'!A24:L30" display="SinglePhaseZIPLoad"/>
@@ -4027,27 +4086,27 @@
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="4" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="4" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="4" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" s="4" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="4" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -4088,7 +4147,7 @@
     </row>
     <row r="11" spans="1:8">
       <c r="A11" s="1" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="B11" s="1"/>
       <c r="C11" s="4" t="s">
@@ -4103,29 +4162,29 @@
         <v>228</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="G12" s="7" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
     </row>
     <row r="13" spans="1:8">
       <c r="A13" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
     </row>
     <row r="15" spans="1:8">
       <c r="A15" s="1" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="B15" s="1"/>
       <c r="C15" s="4" t="s">
@@ -4140,27 +4199,27 @@
         <v>228</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="F16" s="7" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="G16" s="7" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="H16" s="7" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
     </row>
     <row r="17" spans="1:27">
       <c r="A17" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="B17">
         <v>1</v>
@@ -4175,18 +4234,18 @@
         <v>147</v>
       </c>
       <c r="F17" s="9">
-        <v>0.5111219227746321</v>
+        <v>0.2485484768</v>
       </c>
       <c r="G17" s="9">
-        <v>0.5239016640804961</v>
+        <v>0.8699196688</v>
       </c>
       <c r="H17" s="9">
-        <v>1.801475010248056</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:27">
       <c r="A18" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="B18">
         <v>1</v>
@@ -4212,12 +4271,12 @@
     </row>
     <row r="19" spans="1:27">
       <c r="A19" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
     </row>
     <row r="21" spans="1:27">
       <c r="A21" s="1" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="B21" s="1"/>
       <c r="C21" s="4" t="s">
@@ -4232,51 +4291,51 @@
         <v>228</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="D22" s="7" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="E22" s="7" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="F22" s="7" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="G22" s="7" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="H22" s="7" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="I22" s="7" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="J22" s="7" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="K22" s="7" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="L22" s="7" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="M22" s="7" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="N22" s="7" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="O22" s="7" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="P22" s="7" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
     </row>
     <row r="23" spans="1:27">
       <c r="A23" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="B23">
         <v>1</v>
@@ -4297,36 +4356,36 @@
         <v>160</v>
       </c>
       <c r="H23" s="9">
-        <v>0.513284294522792</v>
+        <v>0.2485484768</v>
       </c>
       <c r="I23" s="9">
-        <v>0.520118134892408</v>
+        <v>0.8699196688</v>
       </c>
       <c r="J23" s="9">
-        <v>0.07976914814419199</v>
+        <v>0</v>
       </c>
       <c r="K23" s="9">
-        <v>0.177259802684224</v>
+        <v>0</v>
       </c>
       <c r="L23" s="9">
-        <v>0.5111219227746321</v>
+        <v>0.2485484768</v>
       </c>
       <c r="M23" s="9">
-        <v>0.5239016640804961</v>
+        <v>0.8699196688</v>
       </c>
       <c r="N23" s="9">
-        <v>1.818424773623432</v>
+        <v>0</v>
       </c>
       <c r="O23" s="9">
-        <v>-0.347453372173024</v>
+        <v>0</v>
       </c>
       <c r="P23" s="9">
-        <v>1.801475010248056</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:27">
       <c r="A24" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="B24">
         <v>1</v>
@@ -4347,36 +4406,36 @@
         <v>162</v>
       </c>
       <c r="H24" s="9">
-        <v>0.513284294522792</v>
+        <v>0.2485484768</v>
       </c>
       <c r="I24" s="9">
-        <v>0.520118134892408</v>
+        <v>0.8699196688</v>
       </c>
       <c r="J24" s="9">
-        <v>0.07976914814419199</v>
+        <v>0</v>
       </c>
       <c r="K24" s="9">
-        <v>0.177259802684224</v>
+        <v>0</v>
       </c>
       <c r="L24" s="9">
-        <v>0.5111219227746321</v>
+        <v>0.2485484768</v>
       </c>
       <c r="M24" s="9">
-        <v>0.5239016640804961</v>
+        <v>0.8699196688</v>
       </c>
       <c r="N24" s="9">
-        <v>1.818424773623432</v>
+        <v>0</v>
       </c>
       <c r="O24" s="9">
-        <v>-0.347453372173024</v>
+        <v>0</v>
       </c>
       <c r="P24" s="9">
-        <v>1.801475010248056</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:27">
       <c r="A25" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="B25">
         <v>1</v>
@@ -4397,10 +4456,10 @@
         <v>181</v>
       </c>
       <c r="H25" s="9">
-        <v>0</v>
+        <v>0.2485484768</v>
       </c>
       <c r="I25" s="9">
-        <v>0</v>
+        <v>0.8699196688</v>
       </c>
       <c r="J25" s="9">
         <v>0</v>
@@ -4409,10 +4468,10 @@
         <v>0</v>
       </c>
       <c r="L25" s="9">
-        <v>0.5111219227746321</v>
+        <v>0.2485484768</v>
       </c>
       <c r="M25" s="9">
-        <v>0.5239016640804961</v>
+        <v>0.8699196688</v>
       </c>
       <c r="N25" s="9">
         <v>0</v>
@@ -4421,17 +4480,17 @@
         <v>0</v>
       </c>
       <c r="P25" s="9">
-        <v>1.801475010248056</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:27">
       <c r="A26" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
     </row>
     <row r="28" spans="1:27">
       <c r="A28" s="1" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="B28" s="1"/>
       <c r="C28" s="4" t="s">
@@ -4446,84 +4505,84 @@
         <v>228</v>
       </c>
       <c r="C29" s="7" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="D29" s="7" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="E29" s="7" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="F29" s="7" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="G29" s="7" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="H29" s="7" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="I29" s="7" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="J29" s="7" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="K29" s="7" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="L29" s="7" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="M29" s="7" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="N29" s="7" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="O29" s="7" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="P29" s="7" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="Q29" s="7" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="R29" s="7" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="S29" s="7" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="T29" s="7" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="U29" s="7" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="V29" s="7" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="W29" s="7" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="X29" s="7" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="Y29" s="7" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="Z29" s="7" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="AA29" s="7" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
     </row>
     <row r="30" spans="1:27">
       <c r="A30" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="B30">
         <v>1</v>
@@ -4550,63 +4609,63 @@
         <v>152</v>
       </c>
       <c r="J30" s="9">
-        <v>0.13378432449356</v>
+        <v>0.2485484768</v>
       </c>
       <c r="K30" s="9">
-        <v>0.393013550712848</v>
+        <v>0.8699196688</v>
       </c>
       <c r="L30" s="9">
-        <v>0.06015494509752</v>
+        <v>0</v>
       </c>
       <c r="M30" s="9">
-        <v>0.168610937062776</v>
+        <v>0</v>
       </c>
       <c r="N30" s="9">
-        <v>0.130309616787896</v>
+        <v>0.2485484768</v>
       </c>
       <c r="O30" s="9">
-        <v>0.404557384717824</v>
+        <v>0.8699196688</v>
       </c>
       <c r="P30" s="9">
-        <v>0.06015494509752</v>
+        <v>0</v>
       </c>
       <c r="Q30" s="9">
-        <v>0.168610937062776</v>
+        <v>0</v>
       </c>
       <c r="R30" s="9">
-        <v>0.06015494509752</v>
+        <v>0</v>
       </c>
       <c r="S30" s="9">
-        <v>0.168610937062776</v>
+        <v>0</v>
       </c>
       <c r="T30" s="9">
-        <v>0.131815199186112</v>
+        <v>0.2485484768</v>
       </c>
       <c r="U30" s="9">
-        <v>0.39953856960004</v>
+        <v>0.8699196688</v>
       </c>
       <c r="V30" s="9">
-        <v>2.432365608909496</v>
+        <v>0</v>
       </c>
       <c r="W30" s="9">
-        <v>-0.514404005410776</v>
+        <v>0</v>
       </c>
       <c r="X30" s="9">
-        <v>2.30105247764652</v>
+        <v>0</v>
       </c>
       <c r="Y30" s="9">
-        <v>-0.514404005410776</v>
+        <v>0</v>
       </c>
       <c r="Z30" s="9">
-        <v>-0.514404005410776</v>
+        <v>0</v>
       </c>
       <c r="AA30">
-        <v>2.177074633305104</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:27">
       <c r="A31" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="B31">
         <v>1</v>
@@ -4633,63 +4692,63 @@
         <v>173</v>
       </c>
       <c r="J31" s="9">
-        <v>0.13378432449356</v>
+        <v>0.2485484768</v>
       </c>
       <c r="K31" s="9">
-        <v>0.393013550712848</v>
+        <v>0.8699196688</v>
       </c>
       <c r="L31" s="9">
-        <v>0.06015494509752</v>
+        <v>0</v>
       </c>
       <c r="M31" s="9">
-        <v>0.168610937062776</v>
+        <v>0</v>
       </c>
       <c r="N31" s="9">
-        <v>0.130309616787896</v>
+        <v>0.2485484768</v>
       </c>
       <c r="O31" s="9">
-        <v>0.404557384717824</v>
+        <v>0.8699196688</v>
       </c>
       <c r="P31" s="9">
-        <v>0.06015494509752</v>
+        <v>0</v>
       </c>
       <c r="Q31" s="9">
-        <v>0.168610937062776</v>
+        <v>0</v>
       </c>
       <c r="R31" s="9">
-        <v>0.06015494509752</v>
+        <v>0</v>
       </c>
       <c r="S31" s="9">
-        <v>0.168610937062776</v>
+        <v>0</v>
       </c>
       <c r="T31" s="9">
-        <v>0.131815199186112</v>
+        <v>0.2485484768</v>
       </c>
       <c r="U31" s="9">
-        <v>0.39953856960004</v>
+        <v>0.8699196688</v>
       </c>
       <c r="V31" s="9">
-        <v>2.432365608909496</v>
+        <v>0</v>
       </c>
       <c r="W31" s="9">
-        <v>-0.514404005410776</v>
+        <v>0</v>
       </c>
       <c r="X31" s="9">
-        <v>2.30105247764652</v>
+        <v>0</v>
       </c>
       <c r="Y31" s="9">
-        <v>-0.514404005410776</v>
+        <v>0</v>
       </c>
       <c r="Z31" s="9">
-        <v>-0.514404005410776</v>
+        <v>0</v>
       </c>
       <c r="AA31">
-        <v>2.177074633305104</v>
+        <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:27">
       <c r="A32" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="B32">
         <v>1</v>
@@ -4716,63 +4775,63 @@
         <v>155</v>
       </c>
       <c r="J32" s="9">
-        <v>0.13378432449356</v>
+        <v>0.2485484768</v>
       </c>
       <c r="K32" s="9">
-        <v>0.393013550712848</v>
+        <v>0.8699196688</v>
       </c>
       <c r="L32" s="9">
-        <v>0.06015494509752</v>
+        <v>0</v>
       </c>
       <c r="M32" s="9">
-        <v>0.168610937062776</v>
+        <v>0</v>
       </c>
       <c r="N32" s="9">
-        <v>0.130309616787896</v>
+        <v>0.2485484768</v>
       </c>
       <c r="O32" s="9">
-        <v>0.404557384717824</v>
+        <v>0.8699196688</v>
       </c>
       <c r="P32" s="9">
-        <v>0.06015494509752</v>
+        <v>0</v>
       </c>
       <c r="Q32" s="9">
-        <v>0.168610937062776</v>
+        <v>0</v>
       </c>
       <c r="R32" s="9">
-        <v>0.06015494509752</v>
+        <v>0</v>
       </c>
       <c r="S32" s="9">
-        <v>0.168610937062776</v>
+        <v>0</v>
       </c>
       <c r="T32" s="9">
-        <v>0.131815199186112</v>
+        <v>0.2485484768</v>
       </c>
       <c r="U32" s="9">
-        <v>0.39953856960004</v>
+        <v>0.8699196688</v>
       </c>
       <c r="V32" s="9">
-        <v>2.432365608909496</v>
+        <v>0</v>
       </c>
       <c r="W32" s="9">
-        <v>-0.514404005410776</v>
+        <v>0</v>
       </c>
       <c r="X32" s="9">
-        <v>2.30105247764652</v>
+        <v>0</v>
       </c>
       <c r="Y32" s="9">
-        <v>-0.514404005410776</v>
+        <v>0</v>
       </c>
       <c r="Z32" s="9">
-        <v>-0.514404005410776</v>
+        <v>0</v>
       </c>
       <c r="AA32">
-        <v>2.177074633305104</v>
+        <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:27">
       <c r="A33" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="B33">
         <v>1</v>
@@ -4855,7 +4914,7 @@
     </row>
     <row r="34" spans="1:27">
       <c r="A34" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="B34">
         <v>1</v>
@@ -4882,68 +4941,68 @@
         <v>179</v>
       </c>
       <c r="J34" s="9">
-        <v>0.13378432449356</v>
+        <v>0.2485484768</v>
       </c>
       <c r="K34" s="9">
-        <v>0.393013550712848</v>
+        <v>0.8699196688</v>
       </c>
       <c r="L34" s="9">
-        <v>0.06015494509752</v>
+        <v>0</v>
       </c>
       <c r="M34" s="9">
-        <v>0.168610937062776</v>
+        <v>0</v>
       </c>
       <c r="N34" s="9">
-        <v>0.130309616787896</v>
+        <v>0.2485484768</v>
       </c>
       <c r="O34" s="9">
-        <v>0.404557384717824</v>
+        <v>0.8699196688</v>
       </c>
       <c r="P34" s="9">
-        <v>0.06015494509752</v>
+        <v>0</v>
       </c>
       <c r="Q34" s="9">
-        <v>0.168610937062776</v>
+        <v>0</v>
       </c>
       <c r="R34" s="9">
-        <v>0.06015494509752</v>
+        <v>0</v>
       </c>
       <c r="S34" s="9">
-        <v>0.168610937062776</v>
+        <v>0</v>
       </c>
       <c r="T34" s="9">
-        <v>0.131815199186112</v>
+        <v>0.2485484768</v>
       </c>
       <c r="U34" s="9">
-        <v>0.39953856960004</v>
+        <v>0.8699196688</v>
       </c>
       <c r="V34" s="9">
-        <v>2.432365608909496</v>
+        <v>0</v>
       </c>
       <c r="W34" s="9">
-        <v>-0.514404005410776</v>
+        <v>0</v>
       </c>
       <c r="X34" s="9">
-        <v>2.30105247764652</v>
+        <v>0</v>
       </c>
       <c r="Y34" s="9">
-        <v>-0.514404005410776</v>
+        <v>0</v>
       </c>
       <c r="Z34" s="9">
-        <v>-0.514404005410776</v>
+        <v>0</v>
       </c>
       <c r="AA34">
-        <v>2.177074633305104</v>
+        <v>0</v>
       </c>
     </row>
     <row r="35" spans="1:27">
       <c r="A35" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
     </row>
     <row r="37" spans="1:27">
       <c r="A37" s="1" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="B37" s="1"/>
       <c r="C37" s="4" t="s">
@@ -4958,48 +5017,48 @@
         <v>228</v>
       </c>
       <c r="C38" s="7" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="D38" s="7" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="E38" s="7" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="F38" s="7" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="G38" s="7" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="H38" s="7" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="I38" s="7" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="J38" s="7" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="K38" s="7" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="L38" s="7" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="M38" s="7" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="N38" s="7" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="O38" s="7" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
     </row>
     <row r="39" spans="1:27">
       <c r="A39" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
     </row>
   </sheetData>
@@ -5064,22 +5123,22 @@
     </row>
     <row r="2" spans="1:19">
       <c r="A2" s="4" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
     </row>
     <row r="3" spans="1:19">
       <c r="A3" s="4" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
     </row>
     <row r="4" spans="1:19">
       <c r="A4" s="4" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
     </row>
     <row r="5" spans="1:19">
       <c r="A5" s="4" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
     </row>
     <row r="8" spans="1:19">
@@ -5120,7 +5179,7 @@
     </row>
     <row r="11" spans="1:19">
       <c r="A11" s="1" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -5136,41 +5195,41 @@
         <v>228</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="G12" s="7" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="H12" s="7" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="I12" s="7" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="J12" s="7" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="K12" s="7" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
     </row>
     <row r="13" spans="1:19">
       <c r="A13" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
     </row>
     <row r="15" spans="1:19">
       <c r="A15" s="1" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -5195,56 +5254,56 @@
         <v>208</v>
       </c>
       <c r="F16" s="7" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="G16" s="7" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="H16" s="7" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="I16" s="7" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="J16" s="7" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="K16" s="7" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="L16" s="7" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="M16" s="7" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="N16" s="7" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="O16" s="7" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="P16" s="7" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="Q16" s="7" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="R16" s="7" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="S16" s="7" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
     </row>
     <row r="17" spans="1:27">
       <c r="A17" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
     </row>
     <row r="19" spans="1:27">
       <c r="A19" s="1" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -5260,7 +5319,7 @@
         <v>228</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="D20" s="7" t="s">
         <v>201</v>
@@ -5275,7 +5334,7 @@
         <v>237</v>
       </c>
       <c r="H20" s="7" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="I20" s="7" t="s">
         <v>239</v>
@@ -5293,45 +5352,45 @@
         <v>237</v>
       </c>
       <c r="N20" s="7" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="O20" s="7" t="s">
         <v>239</v>
       </c>
       <c r="P20" s="7" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="Q20" s="7" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="R20" s="7" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="S20" s="7" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="T20" s="7" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="U20" s="7" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="V20" s="7" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="W20" s="7" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="X20" s="7" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="Y20" s="7" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
     </row>
     <row r="21" spans="1:27">
       <c r="A21" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="B21" s="3">
         <v>1</v>
@@ -5381,6 +5440,9 @@
       <c r="Q21" s="2">
         <v>1</v>
       </c>
+      <c r="R21" s="2">
+        <v>1</v>
+      </c>
       <c r="W21" s="10">
         <v>0.02</v>
       </c>
@@ -5393,12 +5455,12 @@
     </row>
     <row r="22" spans="1:27">
       <c r="A22" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
     </row>
     <row r="24" spans="1:27">
       <c r="A24" s="1" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
@@ -5414,7 +5476,7 @@
         <v>228</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="D25" s="7" t="s">
         <v>201</v>
@@ -5429,7 +5491,7 @@
         <v>237</v>
       </c>
       <c r="H25" s="7" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="I25" s="7" t="s">
         <v>239</v>
@@ -5447,51 +5509,51 @@
         <v>237</v>
       </c>
       <c r="N25" s="7" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="O25" s="7" t="s">
         <v>239</v>
       </c>
       <c r="P25" s="7" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="Q25" s="7" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="R25" s="7" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="S25" s="7" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="T25" s="7" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="U25" s="7" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="V25" s="7" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="W25" s="7" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="X25" s="7" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="Y25" s="7" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="Z25" s="7" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="AA25" s="7" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
     </row>
     <row r="26" spans="1:27">
       <c r="A26" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
     </row>
   </sheetData>
@@ -5524,6 +5586,122 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="2" width="18.7109375" customWidth="1"/>
+    <col min="3" max="3" width="28.7109375" customWidth="1"/>
+    <col min="4" max="4" width="8.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>374</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>163</v>
+      </c>
+      <c r="B2" t="s">
+        <v>167</v>
+      </c>
+      <c r="C2" t="s">
+        <v>375</v>
+      </c>
+      <c r="D2" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>165</v>
+      </c>
+      <c r="B3" t="s">
+        <v>168</v>
+      </c>
+      <c r="C3" t="s">
+        <v>376</v>
+      </c>
+      <c r="D3" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>166</v>
+      </c>
+      <c r="B4" t="s">
+        <v>169</v>
+      </c>
+      <c r="C4" t="s">
+        <v>377</v>
+      </c>
+      <c r="D4" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
+        <v>171</v>
+      </c>
+      <c r="B5" t="s">
+        <v>182</v>
+      </c>
+      <c r="C5" t="s">
+        <v>378</v>
+      </c>
+      <c r="D5" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" t="s">
+        <v>172</v>
+      </c>
+      <c r="B6" t="s">
+        <v>183</v>
+      </c>
+      <c r="C6" t="s">
+        <v>379</v>
+      </c>
+      <c r="D6" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" t="s">
+        <v>173</v>
+      </c>
+      <c r="B7" t="s">
+        <v>184</v>
+      </c>
+      <c r="C7" t="s">
+        <v>380</v>
+      </c>
+      <c r="D7" s="3">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:N27"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -5542,22 +5720,22 @@
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="4" t="s">
-        <v>372</v>
+        <v>381</v>
       </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="4" t="s">
-        <v>373</v>
+        <v>382</v>
       </c>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="4" t="s">
-        <v>374</v>
+        <v>383</v>
       </c>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" s="4" t="s">
-        <v>375</v>
+        <v>384</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -5598,7 +5776,7 @@
     </row>
     <row r="11" spans="1:8">
       <c r="A11" s="1" t="s">
-        <v>376</v>
+        <v>385</v>
       </c>
       <c r="B11" s="1"/>
       <c r="C11" s="4" t="s">
@@ -5624,12 +5802,12 @@
     </row>
     <row r="13" spans="1:8">
       <c r="A13" t="s">
-        <v>377</v>
+        <v>386</v>
       </c>
     </row>
     <row r="15" spans="1:8">
       <c r="A15" s="1" t="s">
-        <v>378</v>
+        <v>387</v>
       </c>
       <c r="B15" s="1"/>
       <c r="C15" s="4" t="s">
@@ -5644,7 +5822,7 @@
         <v>228</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>379</v>
+        <v>388</v>
       </c>
       <c r="D16" s="7" t="s">
         <v>201</v>
@@ -5658,7 +5836,7 @@
     </row>
     <row r="17" spans="1:14">
       <c r="A17" t="s">
-        <v>380</v>
+        <v>389</v>
       </c>
       <c r="B17" s="3">
         <v>1</v>
@@ -5678,12 +5856,12 @@
     </row>
     <row r="18" spans="1:14">
       <c r="A18" t="s">
-        <v>381</v>
+        <v>390</v>
       </c>
     </row>
     <row r="20" spans="1:14">
       <c r="A20" s="1" t="s">
-        <v>382</v>
+        <v>391</v>
       </c>
       <c r="B20" s="1"/>
       <c r="C20" s="4" t="s">
@@ -5695,13 +5873,13 @@
         <v>194</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>383</v>
+        <v>392</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>384</v>
+        <v>393</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>379</v>
+        <v>388</v>
       </c>
       <c r="E21" s="7" t="s">
         <v>201</v>
@@ -5724,12 +5902,12 @@
     </row>
     <row r="22" spans="1:14">
       <c r="A22" t="s">
-        <v>385</v>
+        <v>394</v>
       </c>
     </row>
     <row r="24" spans="1:14">
       <c r="A24" s="1" t="s">
-        <v>386</v>
+        <v>395</v>
       </c>
       <c r="B24" s="1"/>
       <c r="C24" s="4" t="s">
@@ -5741,16 +5919,16 @@
         <v>194</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>383</v>
+        <v>392</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>384</v>
+        <v>393</v>
       </c>
       <c r="D25" s="7" t="s">
-        <v>387</v>
+        <v>396</v>
       </c>
       <c r="E25" s="7" t="s">
-        <v>379</v>
+        <v>388</v>
       </c>
       <c r="F25" s="7" t="s">
         <v>201</v>
@@ -5782,7 +5960,7 @@
     </row>
     <row r="26" spans="1:14">
       <c r="A26" t="s">
-        <v>388</v>
+        <v>397</v>
       </c>
       <c r="B26" s="3">
         <v>1</v>
@@ -5826,7 +6004,7 @@
     </row>
     <row r="27" spans="1:14">
       <c r="A27" t="s">
-        <v>389</v>
+        <v>398</v>
       </c>
     </row>
   </sheetData>
@@ -5855,120 +6033,4 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="2" width="18.7109375" customWidth="1"/>
-    <col min="3" max="3" width="28.7109375" customWidth="1"/>
-    <col min="4" max="4" width="8.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" s="1" t="s">
-        <v>390</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>391</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>194</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2" t="s">
-        <v>163</v>
-      </c>
-      <c r="B2" t="s">
-        <v>167</v>
-      </c>
-      <c r="C2" t="s">
-        <v>392</v>
-      </c>
-      <c r="D2" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" t="s">
-        <v>165</v>
-      </c>
-      <c r="B3" t="s">
-        <v>168</v>
-      </c>
-      <c r="C3" t="s">
-        <v>393</v>
-      </c>
-      <c r="D3" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" t="s">
-        <v>166</v>
-      </c>
-      <c r="B4" t="s">
-        <v>169</v>
-      </c>
-      <c r="C4" t="s">
-        <v>394</v>
-      </c>
-      <c r="D4" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5" t="s">
-        <v>171</v>
-      </c>
-      <c r="B5" t="s">
-        <v>182</v>
-      </c>
-      <c r="C5" t="s">
-        <v>395</v>
-      </c>
-      <c r="D5" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6" t="s">
-        <v>172</v>
-      </c>
-      <c r="B6" t="s">
-        <v>183</v>
-      </c>
-      <c r="C6" t="s">
-        <v>396</v>
-      </c>
-      <c r="D6" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="A7" t="s">
-        <v>173</v>
-      </c>
-      <c r="B7" t="s">
-        <v>184</v>
-      </c>
-      <c r="C7" t="s">
-        <v>397</v>
-      </c>
-      <c r="D7" s="3">
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>